<commit_message>
bug fixes and enhancements
</commit_message>
<xml_diff>
--- a/Tasks To Complete.xlsx
+++ b/Tasks To Complete.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="11145" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="11145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ADMIN UI" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -238,11 +244,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +554,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,13 +672,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -680,13 +687,13 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -770,13 +777,13 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -812,6 +819,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1062,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,13 +1099,13 @@
         <f>1+A2</f>
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1106,13 +1114,13 @@
         <f t="shared" ref="A4:A8" si="0">1+A3</f>
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1185,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1226,7 +1234,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A9" si="0">1+A3</f>
+        <f t="shared" ref="A4:A6" si="0">1+A3</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">

</xml_diff>

<commit_message>
firebase finialization and clientui features
</commit_message>
<xml_diff>
--- a/Tasks To Complete.xlsx
+++ b/Tasks To Complete.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="69">
   <si>
     <t>TASK</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>Modify Placed online orders</t>
+  </si>
+  <si>
+    <t>thaniga</t>
+  </si>
+  <si>
+    <t>christen</t>
+  </si>
+  <si>
+    <t>Dhamu</t>
   </si>
 </sst>
 </file>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +617,7 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -622,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
         <v>1</v>
@@ -636,8 +645,11 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A18" si="0">1+A3</f>
         <v>2</v>
@@ -651,8 +663,11 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -667,7 +682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -681,8 +696,11 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -697,7 +715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -712,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -727,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -742,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -757,7 +775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -772,7 +790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -787,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -802,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -817,7 +835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -832,7 +850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -847,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -862,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -876,7 +894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -890,7 +908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -904,7 +922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -918,7 +936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -932,7 +950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -946,7 +964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -959,8 +977,11 @@
       <c r="D25" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -984,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C17" sqref="A17:C17"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feature toggle and search products action
</commit_message>
<xml_diff>
--- a/Tasks To Complete.xlsx
+++ b/Tasks To Complete.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="100">
   <si>
     <t>TASK</t>
   </si>
@@ -300,6 +300,24 @@
   </si>
   <si>
     <t>Pagination for pos &amp; order history</t>
+  </si>
+  <si>
+    <t>Christen</t>
+  </si>
+  <si>
+    <t>alerts &amp; ui fields check</t>
+  </si>
+  <si>
+    <t>OTP functionality</t>
+  </si>
+  <si>
+    <t>Move Search tab to separate component</t>
+  </si>
+  <si>
+    <t>Add/edit address in profile tab</t>
+  </si>
+  <si>
+    <t>Sorting and pagination for searched products</t>
   </si>
 </sst>
 </file>
@@ -322,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +389,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -384,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -394,6 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -1420,17 +1445,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="51.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1867,9 +1892,74 @@
       <c r="H19" t="s">
         <v>18</v>
       </c>
+      <c r="I19" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>